<commit_message>
implemented method2 but have GUI problem
</commit_message>
<xml_diff>
--- a/fixtures/input/emisloc.xlsx
+++ b/fixtures/input/emisloc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\com\sca\hem4\fixtures\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM4\fixtures\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235B4EE7-0274-40BB-82FF-8EE507AEFBE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35168C8-E68F-41F9-85A9-D723388EED57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4EEE6A0-0354-4C0A-A347-EF3D1D72A6CF}"/>
+    <workbookView xWindow="528" yWindow="168" windowWidth="22512" windowHeight="12156" xr2:uid="{B4EEE6A0-0354-4C0A-A347-EF3D1D72A6CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>FacilityID</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Massfrac</t>
+  </si>
+  <si>
+    <t>Partdiam</t>
   </si>
 </sst>
 </file>
@@ -138,10 +147,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,15 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EECB63-0A00-4876-B35C-BE955EDD2460}">
-  <dimension ref="A2:T3"/>
+  <dimension ref="A2:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,8 +536,17 @@
       <c r="T2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -570,6 +589,15 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>0.04</v>
+      </c>
+      <c r="W3">
+        <v>5.9999999999999995E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>